<commit_message>
Various updates to all of the databases and code based on working on failures for Test PIV-I
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV-I_Production_Cards.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV-I_Production_Cards.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\conformancelib\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GSA\GSA_GIT\piv-conformance-pkix-11\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC2562E5-5A77-40B4-BB02-77E2C7079707}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99035DF0-8C32-4F08-8CC6-09D1C78BD672}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="26190" windowHeight="13845" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3755" uniqueCount="1309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3752" uniqueCount="1309">
   <si>
     <t>BER_TLV_Test_Assertions</t>
   </si>
@@ -8516,10 +8516,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:G470"/>
+  <dimension ref="A1:G469"/>
   <sheetViews>
-    <sheetView topLeftCell="A108" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F112" sqref="F112"/>
+    <sheetView tabSelected="1" topLeftCell="A418" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A429" sqref="A429:XFD429"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -13222,7 +13222,7 @@
       <c r="F261" s="39"/>
       <c r="G261" s="43"/>
     </row>
-    <row r="262" spans="1:7" ht="60">
+    <row r="262" spans="1:7" ht="75">
       <c r="A262" s="39" t="s">
         <v>56</v>
       </c>
@@ -13375,7 +13375,7 @@
       <c r="F270" s="40"/>
       <c r="G270" s="40"/>
     </row>
-    <row r="271" spans="1:7" ht="60">
+    <row r="271" spans="1:7" ht="75">
       <c r="A271" s="39" t="s">
         <v>56</v>
       </c>
@@ -13629,7 +13629,9 @@
         <v>485</v>
       </c>
       <c r="E285" s="39"/>
-      <c r="F285" s="39"/>
+      <c r="F285" s="39" t="s">
+        <v>1126</v>
+      </c>
       <c r="G285" s="43"/>
     </row>
     <row r="286" spans="1:7" ht="75">
@@ -13679,7 +13681,7 @@
       <c r="F288" s="40"/>
       <c r="G288" s="40"/>
     </row>
-    <row r="289" spans="1:7" ht="60">
+    <row r="289" spans="1:7" ht="75">
       <c r="A289" s="39" t="s">
         <v>56</v>
       </c>
@@ -13933,7 +13935,9 @@
         <v>485</v>
       </c>
       <c r="E303" s="39"/>
-      <c r="F303" s="39"/>
+      <c r="F303" s="39" t="s">
+        <v>1126</v>
+      </c>
       <c r="G303" s="43"/>
     </row>
     <row r="304" spans="1:7" ht="75">
@@ -14036,7 +14040,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="310" spans="1:7">
+    <row r="310" spans="1:7" ht="30">
       <c r="A310" s="39" t="s">
         <v>56</v>
       </c>
@@ -14070,7 +14074,7 @@
       <c r="F311" s="39"/>
       <c r="G311" s="43"/>
     </row>
-    <row r="312" spans="1:7" ht="45">
+    <row r="312" spans="1:7" ht="60">
       <c r="A312" s="39" t="s">
         <v>56</v>
       </c>
@@ -14168,7 +14172,7 @@
       <c r="F317" s="40"/>
       <c r="G317" s="48"/>
     </row>
-    <row r="318" spans="1:7" ht="60">
+    <row r="318" spans="1:7" ht="75">
       <c r="A318" s="39" t="s">
         <v>56</v>
       </c>
@@ -14422,7 +14426,9 @@
         <v>485</v>
       </c>
       <c r="E332" s="39"/>
-      <c r="F332" s="39"/>
+      <c r="F332" s="39" t="s">
+        <v>1126</v>
+      </c>
       <c r="G332" s="39"/>
     </row>
     <row r="333" spans="1:7" ht="75">
@@ -16213,18 +16219,18 @@
       </c>
       <c r="G428" s="39"/>
     </row>
-    <row r="429" spans="1:7">
+    <row r="429" spans="1:7" ht="45">
       <c r="A429" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B429" s="39" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="C429" s="43" t="s">
-        <v>579</v>
+        <v>666</v>
       </c>
       <c r="D429" s="39" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="E429" s="39"/>
       <c r="F429" s="39" t="s">
@@ -16232,49 +16238,51 @@
       </c>
       <c r="G429" s="43"/>
     </row>
-    <row r="430" spans="1:7" ht="45">
+    <row r="430" spans="1:7">
       <c r="A430" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B430" s="39" t="s">
-        <v>710</v>
-      </c>
-      <c r="C430" s="43" t="s">
-        <v>666</v>
-      </c>
-      <c r="D430" s="39" t="s">
-        <v>583</v>
-      </c>
-      <c r="E430" s="39"/>
-      <c r="F430" s="39" t="s">
+        <v>711</v>
+      </c>
+      <c r="C430" s="40" t="s">
+        <v>585</v>
+      </c>
+      <c r="D430" s="40"/>
+      <c r="E430" s="40"/>
+      <c r="F430" s="40"/>
+      <c r="G430" s="40"/>
+    </row>
+    <row r="431" spans="1:7" ht="90">
+      <c r="A431" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B431" s="39" t="s">
+        <v>712</v>
+      </c>
+      <c r="C431" s="43" t="s">
+        <v>588</v>
+      </c>
+      <c r="D431" s="39" t="s">
+        <v>586</v>
+      </c>
+      <c r="E431" s="39"/>
+      <c r="F431" s="39" t="s">
         <v>1182</v>
       </c>
-      <c r="G430" s="43"/>
-    </row>
-    <row r="431" spans="1:7">
-      <c r="A431" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="B431" s="39" t="s">
-        <v>711</v>
-      </c>
-      <c r="C431" s="40" t="s">
-        <v>585</v>
-      </c>
-      <c r="D431" s="40"/>
-      <c r="E431" s="40"/>
-      <c r="F431" s="40"/>
-      <c r="G431" s="40"/>
-    </row>
-    <row r="432" spans="1:7" ht="90">
+      <c r="G431" s="43" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="432" spans="1:7" ht="60">
       <c r="A432" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B432" s="39" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="C432" s="43" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="D432" s="39" t="s">
         <v>586</v>
@@ -16283,19 +16291,17 @@
       <c r="F432" s="39" t="s">
         <v>1182</v>
       </c>
-      <c r="G432" s="43" t="s">
-        <v>1117</v>
-      </c>
-    </row>
-    <row r="433" spans="1:7" ht="60">
+      <c r="G432" s="43"/>
+    </row>
+    <row r="433" spans="1:7" ht="30">
       <c r="A433" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B433" s="39" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="C433" s="43" t="s">
-        <v>590</v>
+        <v>715</v>
       </c>
       <c r="D433" s="39" t="s">
         <v>586</v>
@@ -16304,165 +16310,165 @@
       <c r="F433" s="39" t="s">
         <v>1182</v>
       </c>
-      <c r="G433" s="43"/>
+      <c r="G433" s="43" t="s">
+        <v>586</v>
+      </c>
     </row>
     <row r="434" spans="1:7" ht="30">
       <c r="A434" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B434" s="39" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="C434" s="43" t="s">
-        <v>715</v>
+        <v>668</v>
       </c>
       <c r="D434" s="39" t="s">
-        <v>586</v>
+        <v>598</v>
       </c>
       <c r="E434" s="39"/>
       <c r="F434" s="39" t="s">
         <v>1182</v>
       </c>
-      <c r="G434" s="43" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="435" spans="1:7" ht="30">
+      <c r="G434" s="43"/>
+    </row>
+    <row r="435" spans="1:7">
       <c r="A435" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B435" s="39" t="s">
-        <v>716</v>
-      </c>
-      <c r="C435" s="43" t="s">
-        <v>668</v>
-      </c>
-      <c r="D435" s="39" t="s">
-        <v>598</v>
-      </c>
-      <c r="E435" s="39"/>
-      <c r="F435" s="39" t="s">
-        <v>1182</v>
-      </c>
-      <c r="G435" s="43"/>
+        <v>717</v>
+      </c>
+      <c r="C435" s="40" t="s">
+        <v>600</v>
+      </c>
+      <c r="D435" s="40"/>
+      <c r="E435" s="40"/>
+      <c r="F435" s="40"/>
+      <c r="G435" s="40"/>
     </row>
     <row r="436" spans="1:7">
       <c r="A436" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B436" s="39" t="s">
-        <v>717</v>
-      </c>
-      <c r="C436" s="40" t="s">
-        <v>600</v>
-      </c>
-      <c r="D436" s="40"/>
-      <c r="E436" s="40"/>
-      <c r="F436" s="40"/>
-      <c r="G436" s="40"/>
+        <v>718</v>
+      </c>
+      <c r="C436" s="43" t="s">
+        <v>602</v>
+      </c>
+      <c r="D436" s="39" t="s">
+        <v>577</v>
+      </c>
+      <c r="E436" s="39"/>
+      <c r="F436" s="39" t="s">
+        <v>1182</v>
+      </c>
+      <c r="G436" s="43" t="s">
+        <v>1110</v>
+      </c>
     </row>
     <row r="437" spans="1:7">
       <c r="A437" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B437" s="39" t="s">
-        <v>718</v>
-      </c>
-      <c r="C437" s="43" t="s">
-        <v>602</v>
+        <v>719</v>
+      </c>
+      <c r="C437" s="39" t="s">
+        <v>604</v>
       </c>
       <c r="D437" s="39" t="s">
-        <v>577</v>
-      </c>
-      <c r="E437" s="39"/>
+        <v>1065</v>
+      </c>
+      <c r="E437" s="39" t="s">
+        <v>1221</v>
+      </c>
       <c r="F437" s="39" t="s">
         <v>1182</v>
       </c>
-      <c r="G437" s="43" t="s">
-        <v>1110</v>
-      </c>
+      <c r="G437" s="39"/>
     </row>
     <row r="438" spans="1:7">
       <c r="A438" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B438" s="39" t="s">
-        <v>719</v>
-      </c>
-      <c r="C438" s="39" t="s">
-        <v>604</v>
-      </c>
-      <c r="D438" s="39" t="s">
-        <v>1065</v>
-      </c>
-      <c r="E438" s="39" t="s">
-        <v>1221</v>
-      </c>
-      <c r="F438" s="39" t="s">
+        <v>720</v>
+      </c>
+      <c r="C438" s="40" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D438" s="40"/>
+      <c r="E438" s="40"/>
+      <c r="F438" s="40"/>
+      <c r="G438" s="40"/>
+    </row>
+    <row r="439" spans="1:7" ht="30">
+      <c r="A439" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B439" s="39" t="s">
+        <v>725</v>
+      </c>
+      <c r="C439" s="39" t="s">
+        <v>615</v>
+      </c>
+      <c r="D439" s="39" t="s">
+        <v>1066</v>
+      </c>
+      <c r="E439" s="39" t="s">
+        <v>616</v>
+      </c>
+      <c r="F439" s="39" t="s">
         <v>1182</v>
       </c>
-      <c r="G438" s="39"/>
-    </row>
-    <row r="439" spans="1:7">
-      <c r="A439" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="B439" s="39" t="s">
-        <v>720</v>
-      </c>
-      <c r="C439" s="40" t="s">
-        <v>1075</v>
-      </c>
-      <c r="D439" s="40"/>
-      <c r="E439" s="40"/>
-      <c r="F439" s="40"/>
-      <c r="G439" s="40"/>
-    </row>
-    <row r="440" spans="1:7" ht="30">
+      <c r="G439" s="39"/>
+    </row>
+    <row r="440" spans="1:7">
       <c r="A440" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="B440" s="39" t="s">
-        <v>725</v>
-      </c>
-      <c r="C440" s="39" t="s">
-        <v>615</v>
-      </c>
-      <c r="D440" s="39" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E440" s="39" t="s">
-        <v>616</v>
-      </c>
-      <c r="F440" s="39" t="s">
-        <v>1182</v>
-      </c>
-      <c r="G440" s="39"/>
+      <c r="B440" s="39">
+        <v>11.5</v>
+      </c>
+      <c r="C440" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="D440" s="40"/>
+      <c r="E440" s="40"/>
+      <c r="F440" s="40"/>
+      <c r="G440" s="38"/>
     </row>
     <row r="441" spans="1:7">
       <c r="A441" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="B441" s="39">
-        <v>11.5</v>
-      </c>
-      <c r="C441" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="D441" s="40"/>
-      <c r="E441" s="40"/>
-      <c r="F441" s="40"/>
-      <c r="G441" s="38"/>
+      <c r="B441" s="39" t="s">
+        <v>726</v>
+      </c>
+      <c r="C441" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="D441" s="39"/>
+      <c r="E441" s="43" t="s">
+        <v>268</v>
+      </c>
+      <c r="F441" s="39" t="s">
+        <v>1182</v>
+      </c>
+      <c r="G441" s="43"/>
     </row>
     <row r="442" spans="1:7">
       <c r="A442" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B442" s="39" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="C442" s="43" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D442" s="39"/>
       <c r="E442" s="43" t="s">
@@ -16478,10 +16484,10 @@
         <v>56</v>
       </c>
       <c r="B443" s="39" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="C443" s="43" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D443" s="39"/>
       <c r="E443" s="43" t="s">
@@ -16496,45 +16502,45 @@
       <c r="A444" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="B444" s="39" t="s">
-        <v>728</v>
-      </c>
-      <c r="C444" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="D444" s="39"/>
-      <c r="E444" s="43" t="s">
-        <v>268</v>
-      </c>
-      <c r="F444" s="39" t="s">
-        <v>1182</v>
-      </c>
-      <c r="G444" s="43"/>
+      <c r="B444" s="39">
+        <v>11.6</v>
+      </c>
+      <c r="C444" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D444" s="40"/>
+      <c r="E444" s="38"/>
+      <c r="F444" s="40"/>
+      <c r="G444" s="38"/>
     </row>
     <row r="445" spans="1:7">
       <c r="A445" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="B445" s="39">
-        <v>11.6</v>
-      </c>
-      <c r="C445" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="D445" s="40"/>
-      <c r="E445" s="38"/>
-      <c r="F445" s="40"/>
-      <c r="G445" s="38"/>
+      <c r="B445" s="39" t="s">
+        <v>729</v>
+      </c>
+      <c r="C445" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="D445" s="39"/>
+      <c r="E445" s="43" t="s">
+        <v>268</v>
+      </c>
+      <c r="F445" s="39" t="s">
+        <v>1182</v>
+      </c>
+      <c r="G445" s="43"/>
     </row>
     <row r="446" spans="1:7">
       <c r="A446" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B446" s="39" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="C446" s="43" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D446" s="39"/>
       <c r="E446" s="43" t="s">
@@ -16549,81 +16555,81 @@
       <c r="A447" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="B447" s="39" t="s">
-        <v>730</v>
-      </c>
-      <c r="C447" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="D447" s="39"/>
-      <c r="E447" s="43" t="s">
-        <v>268</v>
-      </c>
-      <c r="F447" s="39" t="s">
-        <v>1182</v>
-      </c>
-      <c r="G447" s="43"/>
+      <c r="B447" s="39">
+        <v>11.7</v>
+      </c>
+      <c r="C447" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="D447" s="40"/>
+      <c r="E447" s="40"/>
+      <c r="F447" s="40"/>
+      <c r="G447" s="38"/>
     </row>
     <row r="448" spans="1:7">
       <c r="A448" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="B448" s="39">
-        <v>11.7</v>
-      </c>
-      <c r="C448" s="38" t="s">
-        <v>51</v>
+      <c r="B448" s="39" t="s">
+        <v>731</v>
+      </c>
+      <c r="C448" s="40" t="s">
+        <v>42</v>
       </c>
       <c r="D448" s="40"/>
       <c r="E448" s="40"/>
       <c r="F448" s="40"/>
-      <c r="G448" s="38"/>
-    </row>
-    <row r="449" spans="1:7">
+      <c r="G448" s="40"/>
+    </row>
+    <row r="449" spans="1:7" ht="105">
       <c r="A449" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B449" s="39" t="s">
-        <v>731</v>
-      </c>
-      <c r="C449" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="D449" s="40"/>
-      <c r="E449" s="40"/>
-      <c r="F449" s="40"/>
-      <c r="G449" s="40"/>
-    </row>
-    <row r="450" spans="1:7" ht="105">
+        <v>732</v>
+      </c>
+      <c r="C449" s="43" t="s">
+        <v>651</v>
+      </c>
+      <c r="D449" s="39">
+        <v>78.3</v>
+      </c>
+      <c r="E449" s="39"/>
+      <c r="F449" s="39" t="s">
+        <v>1126</v>
+      </c>
+      <c r="G449" s="43" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="450" spans="1:7" ht="30">
       <c r="A450" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B450" s="39" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="C450" s="43" t="s">
-        <v>651</v>
+        <v>682</v>
       </c>
       <c r="D450" s="39">
-        <v>78.3</v>
+        <v>78.099999999999994</v>
       </c>
       <c r="E450" s="39"/>
       <c r="F450" s="39" t="s">
         <v>1126</v>
       </c>
-      <c r="G450" s="43" t="s">
-        <v>1107</v>
-      </c>
+      <c r="G450" s="43"/>
     </row>
     <row r="451" spans="1:7" ht="30">
       <c r="A451" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B451" s="39" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="C451" s="43" t="s">
-        <v>682</v>
+        <v>655</v>
       </c>
       <c r="D451" s="39">
         <v>78.099999999999994</v>
@@ -16634,107 +16640,107 @@
       </c>
       <c r="G451" s="43"/>
     </row>
-    <row r="452" spans="1:7" ht="30">
+    <row r="452" spans="1:7">
       <c r="A452" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B452" s="39" t="s">
-        <v>734</v>
-      </c>
-      <c r="C452" s="43" t="s">
-        <v>655</v>
-      </c>
-      <c r="D452" s="39">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="E452" s="39"/>
-      <c r="F452" s="39" t="s">
-        <v>1126</v>
-      </c>
-      <c r="G452" s="43"/>
+        <v>735</v>
+      </c>
+      <c r="C452" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D452" s="40"/>
+      <c r="E452" s="40"/>
+      <c r="F452" s="40"/>
+      <c r="G452" s="40"/>
     </row>
     <row r="453" spans="1:7">
       <c r="A453" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B453" s="39" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="C453" s="40" t="s">
-        <v>43</v>
+        <v>624</v>
       </c>
       <c r="D453" s="40"/>
       <c r="E453" s="40"/>
       <c r="F453" s="40"/>
       <c r="G453" s="40"/>
     </row>
-    <row r="454" spans="1:7">
+    <row r="454" spans="1:7" ht="30">
       <c r="A454" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B454" s="39" t="s">
-        <v>736</v>
-      </c>
-      <c r="C454" s="40" t="s">
-        <v>624</v>
-      </c>
-      <c r="D454" s="40"/>
-      <c r="E454" s="40"/>
-      <c r="F454" s="40"/>
-      <c r="G454" s="40"/>
-    </row>
-    <row r="455" spans="1:7" ht="30">
+        <v>737</v>
+      </c>
+      <c r="C454" s="43" t="s">
+        <v>738</v>
+      </c>
+      <c r="D454" s="39" t="s">
+        <v>557</v>
+      </c>
+      <c r="E454" s="39"/>
+      <c r="F454" s="39" t="s">
+        <v>1126</v>
+      </c>
+      <c r="G454" s="43" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="455" spans="1:7">
       <c r="A455" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B455" s="39" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="C455" s="43" t="s">
-        <v>738</v>
+        <v>690</v>
       </c>
       <c r="D455" s="39" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="E455" s="39"/>
       <c r="F455" s="39" t="s">
         <v>1126</v>
       </c>
-      <c r="G455" s="43" t="s">
-        <v>1118</v>
-      </c>
-    </row>
-    <row r="456" spans="1:7">
+      <c r="G455" s="43"/>
+    </row>
+    <row r="456" spans="1:7" ht="30">
       <c r="A456" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B456" s="39" t="s">
-        <v>739</v>
-      </c>
-      <c r="C456" s="43" t="s">
-        <v>690</v>
+        <v>740</v>
+      </c>
+      <c r="C456" s="39" t="s">
+        <v>741</v>
       </c>
       <c r="D456" s="39" t="s">
-        <v>560</v>
+        <v>1067</v>
       </c>
       <c r="E456" s="39"/>
       <c r="F456" s="39" t="s">
         <v>1126</v>
       </c>
-      <c r="G456" s="43"/>
-    </row>
-    <row r="457" spans="1:7" ht="30">
+      <c r="G456" s="39"/>
+    </row>
+    <row r="457" spans="1:7" ht="45">
       <c r="A457" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B457" s="39" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="C457" s="39" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="D457" s="39" t="s">
-        <v>1067</v>
+        <v>598</v>
       </c>
       <c r="E457" s="39"/>
       <c r="F457" s="39" t="s">
@@ -16742,54 +16748,54 @@
       </c>
       <c r="G457" s="39"/>
     </row>
-    <row r="458" spans="1:7" ht="45">
+    <row r="458" spans="1:7">
       <c r="A458" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B458" s="39" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="C458" s="39" t="s">
-        <v>743</v>
-      </c>
-      <c r="D458" s="39" t="s">
-        <v>598</v>
-      </c>
+        <v>1082</v>
+      </c>
+      <c r="D458" s="39"/>
       <c r="E458" s="39"/>
       <c r="F458" s="39" t="s">
         <v>1126</v>
       </c>
       <c r="G458" s="39"/>
     </row>
-    <row r="459" spans="1:7">
+    <row r="459" spans="1:7" ht="60">
       <c r="A459" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B459" s="39" t="s">
-        <v>744</v>
+        <v>1083</v>
       </c>
       <c r="C459" s="39" t="s">
-        <v>1082</v>
-      </c>
-      <c r="D459" s="39"/>
+        <v>745</v>
+      </c>
+      <c r="D459" s="39" t="s">
+        <v>566</v>
+      </c>
       <c r="E459" s="39"/>
       <c r="F459" s="39" t="s">
         <v>1126</v>
       </c>
       <c r="G459" s="39"/>
     </row>
-    <row r="460" spans="1:7" ht="60">
+    <row r="460" spans="1:7" ht="30">
       <c r="A460" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B460" s="39" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="C460" s="39" t="s">
-        <v>745</v>
+        <v>1081</v>
       </c>
       <c r="D460" s="39" t="s">
-        <v>566</v>
+        <v>700</v>
       </c>
       <c r="E460" s="39"/>
       <c r="F460" s="39" t="s">
@@ -16797,128 +16803,128 @@
       </c>
       <c r="G460" s="39"/>
     </row>
-    <row r="461" spans="1:7" ht="30">
+    <row r="461" spans="1:7">
       <c r="A461" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B461" s="39" t="s">
-        <v>1084</v>
-      </c>
-      <c r="C461" s="39" t="s">
-        <v>1081</v>
-      </c>
-      <c r="D461" s="39" t="s">
-        <v>700</v>
-      </c>
-      <c r="E461" s="39"/>
-      <c r="F461" s="39" t="s">
-        <v>1126</v>
-      </c>
-      <c r="G461" s="39"/>
+        <v>747</v>
+      </c>
+      <c r="C461" s="40" t="s">
+        <v>600</v>
+      </c>
+      <c r="D461" s="40"/>
+      <c r="E461" s="40"/>
+      <c r="F461" s="40"/>
+      <c r="G461" s="40"/>
     </row>
     <row r="462" spans="1:7">
       <c r="A462" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B462" s="39" t="s">
-        <v>747</v>
-      </c>
-      <c r="C462" s="40" t="s">
-        <v>600</v>
-      </c>
-      <c r="D462" s="40"/>
-      <c r="E462" s="40"/>
-      <c r="F462" s="40"/>
-      <c r="G462" s="40"/>
+        <v>748</v>
+      </c>
+      <c r="C462" s="43" t="s">
+        <v>602</v>
+      </c>
+      <c r="D462" s="39" t="s">
+        <v>577</v>
+      </c>
+      <c r="E462" s="39"/>
+      <c r="F462" s="39" t="s">
+        <v>1126</v>
+      </c>
+      <c r="G462" s="43" t="s">
+        <v>1110</v>
+      </c>
     </row>
     <row r="463" spans="1:7">
       <c r="A463" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B463" s="39" t="s">
-        <v>748</v>
-      </c>
-      <c r="C463" s="43" t="s">
-        <v>602</v>
+        <v>749</v>
+      </c>
+      <c r="C463" s="39" t="s">
+        <v>604</v>
       </c>
       <c r="D463" s="39" t="s">
-        <v>577</v>
+        <v>1065</v>
       </c>
       <c r="E463" s="39"/>
       <c r="F463" s="39" t="s">
         <v>1126</v>
       </c>
-      <c r="G463" s="43" t="s">
-        <v>1110</v>
-      </c>
+      <c r="G463" s="39"/>
     </row>
     <row r="464" spans="1:7">
       <c r="A464" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B464" s="39" t="s">
-        <v>749</v>
-      </c>
-      <c r="C464" s="39" t="s">
-        <v>604</v>
-      </c>
-      <c r="D464" s="39" t="s">
-        <v>1065</v>
-      </c>
-      <c r="E464" s="39"/>
-      <c r="F464" s="39" t="s">
-        <v>1126</v>
-      </c>
-      <c r="G464" s="39"/>
+        <v>750</v>
+      </c>
+      <c r="C464" s="40" t="s">
+        <v>606</v>
+      </c>
+      <c r="D464" s="40"/>
+      <c r="E464" s="40"/>
+      <c r="F464" s="40"/>
+      <c r="G464" s="40"/>
     </row>
     <row r="465" spans="1:7">
       <c r="A465" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B465" s="39" t="s">
-        <v>750</v>
-      </c>
-      <c r="C465" s="40" t="s">
-        <v>606</v>
-      </c>
-      <c r="D465" s="40"/>
-      <c r="E465" s="40"/>
-      <c r="F465" s="40"/>
-      <c r="G465" s="40"/>
-    </row>
-    <row r="466" spans="1:7">
+        <v>751</v>
+      </c>
+      <c r="C465" s="43" t="s">
+        <v>570</v>
+      </c>
+      <c r="D465" s="39" t="s">
+        <v>571</v>
+      </c>
+      <c r="E465" s="39"/>
+      <c r="F465" s="39" t="s">
+        <v>1126</v>
+      </c>
+      <c r="G465" s="43" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="466" spans="1:7" ht="30">
       <c r="A466" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B466" s="39" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="C466" s="43" t="s">
-        <v>570</v>
+        <v>645</v>
       </c>
       <c r="D466" s="39" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="E466" s="39"/>
       <c r="F466" s="39" t="s">
         <v>1126</v>
       </c>
-      <c r="G466" s="43" t="s">
-        <v>1119</v>
-      </c>
+      <c r="G466" s="43"/>
     </row>
     <row r="467" spans="1:7" ht="30">
       <c r="A467" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B467" s="39" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="C467" s="43" t="s">
-        <v>645</v>
+        <v>611</v>
       </c>
       <c r="D467" s="39" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="E467" s="39"/>
       <c r="F467" s="39" t="s">
@@ -16926,62 +16932,43 @@
       </c>
       <c r="G467" s="43"/>
     </row>
-    <row r="468" spans="1:7" ht="30">
+    <row r="468" spans="1:7">
       <c r="A468" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B468" s="39" t="s">
-        <v>753</v>
-      </c>
-      <c r="C468" s="43" t="s">
-        <v>611</v>
+        <v>754</v>
+      </c>
+      <c r="C468" s="39" t="s">
+        <v>613</v>
       </c>
       <c r="D468" s="39" t="s">
-        <v>577</v>
+        <v>1068</v>
       </c>
       <c r="E468" s="39"/>
       <c r="F468" s="39" t="s">
         <v>1126</v>
       </c>
-      <c r="G468" s="43"/>
-    </row>
-    <row r="469" spans="1:7">
+      <c r="G468" s="39"/>
+    </row>
+    <row r="469" spans="1:7" ht="30">
       <c r="A469" s="39" t="s">
         <v>56</v>
       </c>
       <c r="B469" s="39" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="C469" s="39" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="D469" s="39" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="E469" s="39"/>
       <c r="F469" s="39" t="s">
         <v>1126</v>
       </c>
       <c r="G469" s="39"/>
-    </row>
-    <row r="470" spans="1:7" ht="30">
-      <c r="A470" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="B470" s="39" t="s">
-        <v>755</v>
-      </c>
-      <c r="C470" s="39" t="s">
-        <v>615</v>
-      </c>
-      <c r="D470" s="39" t="s">
-        <v>1066</v>
-      </c>
-      <c r="E470" s="39"/>
-      <c r="F470" s="39" t="s">
-        <v>1126</v>
-      </c>
-      <c r="G470" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -16994,7 +16981,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AMK6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
@@ -17081,9 +17070,7 @@
       <c r="D4" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>756</v>
-      </c>
+      <c r="E4" s="5"/>
       <c r="F4" s="3" t="s">
         <v>764</v>
       </c>
@@ -17141,7 +17128,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AMK55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>